<commit_message>
Bug Fix 2025/06/27 2
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karst\Dropbox\Research\Dr. Sum\Gas-Hydrate-Equilibrium-Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD1057C-FE8E-4672-A442-6B3EE9354EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7EAD96-9E20-4A12-85D3-718F99614E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11115" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4485" windowWidth="21600" windowHeight="11115" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="3" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="123">
   <si>
     <t>Compound ID</t>
   </si>
@@ -1361,7 +1361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:K2"/>
     </sheetView>
   </sheetViews>
@@ -3349,10 +3349,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5C889D-4057-4DC7-9727-42E8A897B0CB}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3554,36 +3554,36 @@
         <v>0</v>
       </c>
       <c r="C10" s="23">
+        <v>9</v>
+      </c>
+      <c r="D10" s="23">
+        <v>-100</v>
+      </c>
+      <c r="E10" s="23">
+        <v>0</v>
+      </c>
+      <c r="F10" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="23">
+        <v>0</v>
+      </c>
+      <c r="C11" s="23">
         <v>10</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D11" s="23">
         <v>-26.331200055758099</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E11" s="23">
         <v>3822.5148242806899</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F11" s="23">
         <v>-45381.8469139019</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="6">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>-22.06505254</v>
-      </c>
-      <c r="E11">
-        <v>2760.1604400000001</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3594,16 +3594,16 @@
         <v>1</v>
       </c>
       <c r="C12" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>-23.728977069999999</v>
+        <v>-22.06505254</v>
       </c>
       <c r="E12">
-        <v>3843.277306</v>
+        <v>2760.1604400000001</v>
       </c>
       <c r="F12">
-        <v>8882.4254299999993</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3614,16 +3614,16 @@
         <v>1</v>
       </c>
       <c r="C13" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>-100</v>
+        <v>-23.728977069999999</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>3843.277306</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>8882.4254299999993</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3634,13 +3634,13 @@
         <v>1</v>
       </c>
       <c r="C14" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>-21.842441359999999</v>
+        <v>-100</v>
       </c>
       <c r="E14">
-        <v>2337.176449</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -3654,35 +3654,35 @@
         <v>1</v>
       </c>
       <c r="C15" s="6">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>-21.842441359999999</v>
+      </c>
+      <c r="E15">
+        <v>2337.176449</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6">
         <v>5</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>-22.403651719999999</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>3171.7603869999998</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="23">
-        <v>1</v>
-      </c>
-      <c r="C16" s="23">
-        <v>6</v>
-      </c>
-      <c r="D16" s="23">
-        <v>-100</v>
-      </c>
-      <c r="E16" s="23">
-        <v>0</v>
-      </c>
-      <c r="F16" s="23">
+      <c r="F16">
         <v>0</v>
       </c>
     </row>
@@ -3694,7 +3694,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="23">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" s="23">
         <v>-100</v>
@@ -3714,7 +3714,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" s="23">
         <v>-100</v>
@@ -3734,56 +3734,56 @@
         <v>1</v>
       </c>
       <c r="C19" s="23">
+        <v>8</v>
+      </c>
+      <c r="D19" s="23">
+        <v>-100</v>
+      </c>
+      <c r="E19" s="23">
+        <v>0</v>
+      </c>
+      <c r="F19" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="23">
+        <v>1</v>
+      </c>
+      <c r="C20" s="23">
+        <v>9</v>
+      </c>
+      <c r="D20" s="23">
+        <v>-100</v>
+      </c>
+      <c r="E20" s="23">
+        <v>0</v>
+      </c>
+      <c r="F20" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="23">
+        <v>1</v>
+      </c>
+      <c r="C21" s="23">
         <v>10</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D21" s="23">
         <v>-26.921927924317298</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E21" s="23">
         <v>7358.8183572326698</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F21" s="23">
         <v>-237581.84882084699</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="6">
-        <v>0</v>
-      </c>
-      <c r="C20" s="6">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>-23.574602980000002</v>
-      </c>
-      <c r="E20">
-        <v>2708.8070149999999</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="6">
-        <v>0</v>
-      </c>
-      <c r="C21" s="6">
-        <v>2</v>
-      </c>
-      <c r="D21">
-        <v>-24.837826750000001</v>
-      </c>
-      <c r="E21">
-        <v>926.98965250000003</v>
-      </c>
-      <c r="F21">
-        <v>43614.852559999999</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -3794,13 +3794,13 @@
         <v>0</v>
       </c>
       <c r="C22" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>-100</v>
+        <v>-23.574602980000002</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>2708.8070149999999</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -3814,16 +3814,16 @@
         <v>0</v>
       </c>
       <c r="C23" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D23">
-        <v>-22.97258845</v>
+        <v>-24.837826750000001</v>
       </c>
       <c r="E23">
-        <v>2499.2232410000001</v>
+        <v>926.98965250000003</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>43614.852559999999</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -3834,56 +3834,56 @@
         <v>0</v>
       </c>
       <c r="C24" s="6">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>-100</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0</v>
+      </c>
+      <c r="C25" s="6">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>-22.97258845</v>
+      </c>
+      <c r="E25">
+        <v>2499.2232410000001</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="6">
+        <v>0</v>
+      </c>
+      <c r="C26" s="6">
         <v>5</v>
       </c>
-      <c r="D24">
+      <c r="D26">
         <v>-25.175152000000001</v>
       </c>
-      <c r="E24">
+      <c r="E26">
         <v>3089.4741450000001</v>
       </c>
-      <c r="F24">
+      <c r="F26">
         <v>48259.677799999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="23">
-        <v>0</v>
-      </c>
-      <c r="C25" s="23">
-        <v>6</v>
-      </c>
-      <c r="D25" s="23">
-        <v>-100</v>
-      </c>
-      <c r="E25" s="23">
-        <v>0</v>
-      </c>
-      <c r="F25" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="23">
-        <v>0</v>
-      </c>
-      <c r="C26" s="23">
-        <v>7</v>
-      </c>
-      <c r="D26" s="23">
-        <v>-100</v>
-      </c>
-      <c r="E26" s="23">
-        <v>0</v>
-      </c>
-      <c r="F26" s="23">
-        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -3894,7 +3894,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="23">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D27" s="23">
         <v>-100</v>
@@ -3914,76 +3914,76 @@
         <v>0</v>
       </c>
       <c r="C28" s="23">
+        <v>7</v>
+      </c>
+      <c r="D28" s="23">
+        <v>-100</v>
+      </c>
+      <c r="E28" s="23">
+        <v>0</v>
+      </c>
+      <c r="F28" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="23">
+        <v>0</v>
+      </c>
+      <c r="C29" s="23">
+        <v>8</v>
+      </c>
+      <c r="D29" s="23">
+        <v>-100</v>
+      </c>
+      <c r="E29" s="23">
+        <v>0</v>
+      </c>
+      <c r="F29" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="23">
+        <v>0</v>
+      </c>
+      <c r="C30" s="23">
         <v>9</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D30" s="23">
         <v>-22.97258845</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E30" s="23">
         <v>2499.2232410000001</v>
       </c>
-      <c r="F28" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="F30" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="6">
-        <v>1</v>
-      </c>
-      <c r="C29" s="6">
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <v>-20.699072309999998</v>
-      </c>
-      <c r="E29">
-        <v>2147.68986</v>
-      </c>
-      <c r="F29">
-        <v>-12013.621069999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="6">
-        <v>1</v>
-      </c>
-      <c r="C30" s="6">
-        <v>2</v>
-      </c>
-      <c r="D30">
-        <v>-22.229064659999999</v>
-      </c>
-      <c r="E30">
-        <v>3534.8896070000001</v>
-      </c>
-      <c r="F30">
-        <v>-3371.30006</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="6">
-        <v>1</v>
-      </c>
-      <c r="C31" s="6">
-        <v>3</v>
-      </c>
-      <c r="D31">
-        <v>-23.130700000000001</v>
-      </c>
-      <c r="E31">
-        <v>4176.1979000000001</v>
-      </c>
-      <c r="F31">
-        <v>45939.459300000002</v>
+      <c r="B31" s="4">
+        <v>0</v>
+      </c>
+      <c r="C31" s="4">
+        <v>10</v>
+      </c>
+      <c r="D31" s="4">
+        <v>-26.331200055758099</v>
+      </c>
+      <c r="E31" s="4">
+        <v>3822.5148242806899</v>
+      </c>
+      <c r="F31" s="4">
+        <v>-45381.8469139019</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -3994,16 +3994,16 @@
         <v>1</v>
       </c>
       <c r="C32" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D32">
-        <v>-20.615956090000001</v>
+        <v>-20.699072309999998</v>
       </c>
       <c r="E32">
-        <v>2033.604317</v>
+        <v>2147.68986</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>-12013.621069999999</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -4014,76 +4014,76 @@
         <v>1</v>
       </c>
       <c r="C33" s="6">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>-22.229064659999999</v>
+      </c>
+      <c r="E33">
+        <v>3534.8896070000001</v>
+      </c>
+      <c r="F33">
+        <v>-3371.30006</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="6">
+        <v>1</v>
+      </c>
+      <c r="C34" s="6">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>-23.130700000000001</v>
+      </c>
+      <c r="E34">
+        <v>4176.1979000000001</v>
+      </c>
+      <c r="F34">
+        <v>45939.459300000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="6">
+        <v>1</v>
+      </c>
+      <c r="C35" s="6">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>-20.615956090000001</v>
+      </c>
+      <c r="E35">
+        <v>2033.604317</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="6">
+        <v>1</v>
+      </c>
+      <c r="C36" s="6">
         <v>5</v>
       </c>
-      <c r="D33">
+      <c r="D36">
         <v>-21.091724119999999</v>
       </c>
-      <c r="E33">
+      <c r="E36">
         <v>2405.3661569999999</v>
       </c>
-      <c r="F33">
+      <c r="F36">
         <v>28783</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="23">
-        <v>1</v>
-      </c>
-      <c r="C34" s="23">
-        <v>6</v>
-      </c>
-      <c r="D34" s="23">
-        <v>-41.589308423376103</v>
-      </c>
-      <c r="E34" s="23">
-        <v>12568.4056539184</v>
-      </c>
-      <c r="F34" s="23">
-        <v>-984700.06756650598</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="23">
-        <v>1</v>
-      </c>
-      <c r="C35" s="23">
-        <v>7</v>
-      </c>
-      <c r="D35" s="23">
-        <v>-100</v>
-      </c>
-      <c r="E35" s="23">
-        <v>0</v>
-      </c>
-      <c r="F35" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="23">
-        <v>1</v>
-      </c>
-      <c r="C36" s="23">
-        <v>8</v>
-      </c>
-      <c r="D36" s="23">
-        <v>-100</v>
-      </c>
-      <c r="E36" s="23">
-        <v>0</v>
-      </c>
-      <c r="F36" s="23">
-        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -4094,16 +4094,96 @@
         <v>1</v>
       </c>
       <c r="C37" s="23">
+        <v>6</v>
+      </c>
+      <c r="D37" s="23">
+        <v>-41.589308423376103</v>
+      </c>
+      <c r="E37" s="23">
+        <v>12568.4056539184</v>
+      </c>
+      <c r="F37" s="23">
+        <v>-984700.06756650598</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="23">
+        <v>1</v>
+      </c>
+      <c r="C38" s="23">
+        <v>7</v>
+      </c>
+      <c r="D38" s="23">
+        <v>-100</v>
+      </c>
+      <c r="E38" s="23">
+        <v>0</v>
+      </c>
+      <c r="F38" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="23">
+        <v>1</v>
+      </c>
+      <c r="C39" s="23">
+        <v>8</v>
+      </c>
+      <c r="D39" s="23">
+        <v>-100</v>
+      </c>
+      <c r="E39" s="23">
+        <v>0</v>
+      </c>
+      <c r="F39" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="23">
+        <v>1</v>
+      </c>
+      <c r="C40" s="23">
         <v>9</v>
       </c>
-      <c r="D37" s="23">
+      <c r="D40" s="23">
         <v>-20.615956090000001</v>
       </c>
-      <c r="E37" s="23">
+      <c r="E40" s="23">
         <v>2033.604317</v>
       </c>
-      <c r="F37" s="23">
-        <v>0</v>
+      <c r="F40" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="4">
+        <v>1</v>
+      </c>
+      <c r="C41" s="4">
+        <v>10</v>
+      </c>
+      <c r="D41" s="4">
+        <v>-26.921927924317298</v>
+      </c>
+      <c r="E41" s="4">
+        <v>7358.8183572326698</v>
+      </c>
+      <c r="F41" s="4">
+        <v>-237581.84882084699</v>
       </c>
     </row>
   </sheetData>

</xml_diff>